<commit_message>
Progress on step 4: classification and gpt blurb generation complete. Email format needs to change, as well as context around email based on classification. Likely will move classification to validation step, then create blurbs based on those (individual method per generation)
</commit_message>
<xml_diff>
--- a/data_pipelining/input/test_leads.xlsx
+++ b/data_pipelining/input/test_leads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vasumanmoza/Desktop/northpoint/data_pipelining/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B932711-07C3-334E-B78F-A820A722FB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF623A9F-43BD-D141-8454-1454D7D102BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="180">
   <si>
     <t>FIRST NAME</t>
   </si>
@@ -82,12 +82,6 @@
     <t>McNutt</t>
   </si>
   <si>
-    <t>Melissa.McNutt@Samsung.com</t>
-  </si>
-  <si>
-    <t>BOUNCED</t>
-  </si>
-  <si>
     <t>Head of US Marketing @ Inbenta</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>Joshua</t>
   </si>
   <si>
-    <t>JSmith@Salesforce.com</t>
-  </si>
-  <si>
     <t>Head of US Social Marketing for Series and ...</t>
   </si>
   <si>
@@ -112,12 +103,6 @@
     <t>Mills</t>
   </si>
   <si>
-    <t>MMills@Netflix.com</t>
-  </si>
-  <si>
-    <t>EMAIL_SENT</t>
-  </si>
-  <si>
     <t>Health Systems Marketing Lead, Dermatology</t>
   </si>
   <si>
@@ -130,9 +115,6 @@
     <t>Storrs</t>
   </si>
   <si>
-    <t>Christy.Storrs@Pfizer.com</t>
-  </si>
-  <si>
     <t>Helping B2B companies improve Commercial capabilities for Strategic Planning, Marketing, Product and Sales functions.</t>
   </si>
   <si>
@@ -145,9 +127,6 @@
     <t>Wilson</t>
   </si>
   <si>
-    <t>TWilson@Costco.com</t>
-  </si>
-  <si>
     <t>Hematology Marketing Strategy Lead | Pfizer Oncology</t>
   </si>
   <si>
@@ -157,9 +136,6 @@
     <t>PharmD</t>
   </si>
   <si>
-    <t>Wilma.PharmD@Pfizer.com</t>
-  </si>
-  <si>
     <t>High Impact Marketing Leader</t>
   </si>
   <si>
@@ -169,9 +145,6 @@
     <t>Suarez</t>
   </si>
   <si>
-    <t>Tim@Uber.com</t>
-  </si>
-  <si>
     <t>High-Tech Marketing Exec | Inspiring Leader | Animal Advocate | Advisory Board Member</t>
   </si>
   <si>
@@ -184,9 +157,6 @@
     <t>Atterbury</t>
   </si>
   <si>
-    <t>LAtterbury@Paypal.com</t>
-  </si>
-  <si>
     <t>Hiring and Marketing Manager at Phoenix Information Technologies</t>
   </si>
   <si>
@@ -196,9 +166,6 @@
     <t>Foley</t>
   </si>
   <si>
-    <t>MFoley@Paypal.com</t>
-  </si>
-  <si>
     <t>Hiring Top Marketing Talent for disruptive brands</t>
   </si>
   <si>
@@ -211,9 +178,6 @@
     <t>Herbeck</t>
   </si>
   <si>
-    <t>Nicole.Herbeck@Target.com</t>
-  </si>
-  <si>
     <t>Honors Marketing, Psychology, and Entrepreneurship @ SMU | Marketing Consultant at the Intersection of Tech, Gen-Z, and Experiences</t>
   </si>
   <si>
@@ -223,9 +187,6 @@
     <t>Pham</t>
   </si>
   <si>
-    <t>Leon.Pham@Samsung.com</t>
-  </si>
-  <si>
     <t>HR &amp; Marketing Manager</t>
   </si>
   <si>
@@ -235,9 +196,6 @@
     <t>Fischer</t>
   </si>
   <si>
-    <t>Maikely.Fischer@Airbnb.com</t>
-  </si>
-  <si>
     <t>HR Business Partner / Property Management / Hospitality Guru / Sales and Marketing Director/Business Development</t>
   </si>
   <si>
@@ -247,9 +205,6 @@
     <t>Glenn</t>
   </si>
   <si>
-    <t>Brittany.Glenn@Airbnb.com</t>
-  </si>
-  <si>
     <t>HR Marketing Specialist</t>
   </si>
   <si>
@@ -262,9 +217,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Brianna.Price@Marriott.com</t>
-  </si>
-  <si>
     <t>HubSpot Partner | Inbound Marketing | CRM &amp; Sales | Content &amp; eCommerce | ️ Shopify Partner | Google, LinkedIn &amp; Facebook Ads | AI-Powered Digital Marketing | SAP Partners &amp; Customers</t>
   </si>
   <si>
@@ -274,9 +226,6 @@
     <t>Ayers</t>
   </si>
   <si>
-    <t>LAyers@Costco.com</t>
-  </si>
-  <si>
     <t>I create marketing and sales campaigns and copy that generate leads and clients for business coaches, consultants and entrepreneurs. Clients include: Grant Cardone, Copy Chief, Strategic Profits, and Growth Labz</t>
   </si>
   <si>
@@ -286,9 +235,6 @@
     <t>Vaughn</t>
   </si>
   <si>
-    <t>RVaughn@Costco.com</t>
-  </si>
-  <si>
     <t>I Help CEOs Grow Their Startups Up to 17x The Startup CMO Providing Innovative Fractional CMO, Brand &amp; Marketing Services</t>
   </si>
   <si>
@@ -301,18 +247,12 @@
     <t>Volpe</t>
   </si>
   <si>
-    <t>Anthony.Volpe@Fox.com</t>
-  </si>
-  <si>
     <t>I help wellness and health experts attract dream clients with content marketing + personal branding</t>
   </si>
   <si>
     <t>Shtein</t>
   </si>
   <si>
-    <t>HShtein@Netflix.com</t>
-  </si>
-  <si>
     <t>I specialize in helping businesses grow and scale by implementing tailored marketing strategies.</t>
   </si>
   <si>
@@ -322,9 +262,6 @@
     <t>Koreny</t>
   </si>
   <si>
-    <t>SKoreny@Costco.com</t>
-  </si>
-  <si>
     <t>Impossible Foods Marketing Leader | The Marketing Academy 2023 Scholar | Stanford GSB | Coca-Cola</t>
   </si>
   <si>
@@ -337,9 +274,6 @@
     <t>Chapman</t>
   </si>
   <si>
-    <t>SChapman@Coca-Cola.com</t>
-  </si>
-  <si>
     <t>Incoming GOV IT Program Manager @ ALKU | Digital Marketing Student @ Virginia Tech | Co-CMO @ Cornucopia AI</t>
   </si>
   <si>
@@ -349,9 +283,6 @@
     <t>Swain</t>
   </si>
   <si>
-    <t>TSwain@Costco.com</t>
-  </si>
-  <si>
     <t>Incoming Social Marketing Intern</t>
   </si>
   <si>
@@ -361,9 +292,6 @@
     <t>Hartman</t>
   </si>
   <si>
-    <t>EHartman@netflix.com</t>
-  </si>
-  <si>
     <t>Influencer + Integrations Marketing Lead</t>
   </si>
   <si>
@@ -373,9 +301,6 @@
     <t>Christopher</t>
   </si>
   <si>
-    <t>CHill@Spotify.com</t>
-  </si>
-  <si>
     <t>Influencer Marketing</t>
   </si>
   <si>
@@ -385,9 +310,6 @@
     <t>Mitchell</t>
   </si>
   <si>
-    <t>Kiron.Mitchell@Nike.com</t>
-  </si>
-  <si>
     <t>Influencer Marketing @ Dropbox</t>
   </si>
   <si>
@@ -397,39 +319,24 @@
     <t>Roth</t>
   </si>
   <si>
-    <t>Renee.Roth@Fox.com</t>
-  </si>
-  <si>
     <t>Influencer Marketing at PayPal</t>
   </si>
   <si>
     <t>Le</t>
   </si>
   <si>
-    <t>LPham@Paypal.com</t>
-  </si>
-  <si>
     <t>Influencer Marketing Director</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>Alessandra.M@Nike.com</t>
-  </si>
-  <si>
     <t>Influencer Marketing Director for Asia Pacif and Latin America</t>
   </si>
   <si>
     <t>Marder</t>
   </si>
   <si>
-    <t>Alessandra.Marder@Nike.com</t>
-  </si>
-  <si>
-    <t>EMAIL_OPENED</t>
-  </si>
-  <si>
     <t>Influencer Marketing Manager at Unilever Prestige-Ren Clean Skincare</t>
   </si>
   <si>
@@ -439,27 +346,18 @@
     <t>Ameen</t>
   </si>
   <si>
-    <t>Hannah.A@pg.com</t>
-  </si>
-  <si>
     <t>Influencer Marketing Manager, North America Integrated Media</t>
   </si>
   <si>
     <t>Celata</t>
   </si>
   <si>
-    <t>Brittany.Celata@Nike.com</t>
-  </si>
-  <si>
     <t>Influencer Marketing Professional</t>
   </si>
   <si>
     <t>Santos</t>
   </si>
   <si>
-    <t>Joshua.Santos@Fox.com</t>
-  </si>
-  <si>
     <t>Inhouse marketing</t>
   </si>
   <si>
@@ -469,9 +367,6 @@
     <t>Joufrane</t>
   </si>
   <si>
-    <t>Joseph.Joufrane@Marriott.com</t>
-  </si>
-  <si>
     <t>Innovation Channel Alliances, Pfizer Chief Marketing Office</t>
   </si>
   <si>
@@ -481,18 +376,12 @@
     <t>Boukadoum</t>
   </si>
   <si>
-    <t>Elsa.Boukadoum@Pfizer.com</t>
-  </si>
-  <si>
     <t>Innovation Executive in Food &amp; Beverage CPG</t>
   </si>
   <si>
     <t>Phil</t>
   </si>
   <si>
-    <t>Phil.Fox@Fox.com</t>
-  </si>
-  <si>
     <t>Innovation. Customer Insights. Brand Strategy. Marketing Problem Solving.</t>
   </si>
   <si>
@@ -502,9 +391,6 @@
     <t>Peoples</t>
   </si>
   <si>
-    <t>BPeoples@Costco.com</t>
-  </si>
-  <si>
     <t>Innovative Marketing Strategist &amp; Sales Expert | Transforming Businesses with Technology and Automation</t>
   </si>
   <si>
@@ -514,9 +400,6 @@
     <t>DeLaCruz</t>
   </si>
   <si>
-    <t>TDeLaCruz@Costco.com</t>
-  </si>
-  <si>
     <t>Innovative marketing strategy architect</t>
   </si>
   <si>
@@ -526,18 +409,12 @@
     <t>Ainzuain</t>
   </si>
   <si>
-    <t>BAinzuain@Netflix.com</t>
-  </si>
-  <si>
     <t>Innovative, customer-focused marketing leader with 15 years of experience in B2B, B2C, and SMB marketplaces and cloud technology</t>
   </si>
   <si>
     <t>Wang</t>
   </si>
   <si>
-    <t>CWang@Paypal.com</t>
-  </si>
-  <si>
     <t>Insights Driven Marketing Leader | Brand and Media Strategy | previously Airbnb, Netflix, agency</t>
   </si>
   <si>
@@ -547,9 +424,6 @@
     <t>Pirkowski</t>
   </si>
   <si>
-    <t>Rachael.Pirkowski@Airbnb.com</t>
-  </si>
-  <si>
     <t>Inspirational Marketing Leader Delivering ROI</t>
   </si>
   <si>
@@ -559,9 +433,6 @@
     <t>PITT</t>
   </si>
   <si>
-    <t>TPITT@Paypal.com</t>
-  </si>
-  <si>
     <t>Integrated &amp; Multi-Channel Marketing Leader | Data-Driven Strategic Insights</t>
   </si>
   <si>
@@ -571,9 +442,6 @@
     <t>DeMotte</t>
   </si>
   <si>
-    <t>Andrew.DeMotte@ExxonMobil.com</t>
-  </si>
-  <si>
     <t>Integrated Customer Marketing</t>
   </si>
   <si>
@@ -586,9 +454,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>Sabrina.B@Workday.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing @ Meta | Ex- EA, Samsung, Grey</t>
   </si>
   <si>
@@ -598,9 +463,6 @@
     <t>Roberts</t>
   </si>
   <si>
-    <t>Natalie.Roberts@Samsung.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing | Branded Entertainment | Partnership Activation | Campaign Management</t>
   </si>
   <si>
@@ -610,18 +472,12 @@
     <t>Oakes</t>
   </si>
   <si>
-    <t>Martin.Oakes@Fox.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing | Social Media Marketing | Creative Strategist</t>
   </si>
   <si>
     <t>Tristin</t>
   </si>
   <si>
-    <t>Tristin.Brown@Airbnb.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing and Omnichannel Strategist (Consultant)</t>
   </si>
   <si>
@@ -631,9 +487,6 @@
     <t>Stoker</t>
   </si>
   <si>
-    <t>Melinda.Stoker@Pfizer.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing at Ford | EMBA Kellogg</t>
   </si>
   <si>
@@ -643,9 +496,6 @@
     <t>Rainelli</t>
   </si>
   <si>
-    <t>Jaife@Uber.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing Communications Manager</t>
   </si>
   <si>
@@ -655,9 +505,6 @@
     <t>Khan</t>
   </si>
   <si>
-    <t>SKhan@Walmart.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing Manager</t>
   </si>
   <si>
@@ -667,9 +514,6 @@
     <t>Barden</t>
   </si>
   <si>
-    <t>ABarden@netflix.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing Project Manager</t>
   </si>
   <si>
@@ -679,18 +523,12 @@
     <t>Gonzalez</t>
   </si>
   <si>
-    <t>Paula.Gonzalez@Workday.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing Senior Manager at Samsung</t>
   </si>
   <si>
     <t>Wild</t>
   </si>
   <si>
-    <t>Renee.Wild@Samsung.com</t>
-  </si>
-  <si>
     <t>Integrated Marketing Specialist</t>
   </si>
   <si>
@@ -700,9 +538,6 @@
     <t>Ware</t>
   </si>
   <si>
-    <t>Cheyenne.Ware@Nike.com</t>
-  </si>
-  <si>
     <t>Integrated Media Measurement @Coca-Cola | Ex-Meta, Visa, Hershey Co., Agency| Digital Marketing &amp; Media</t>
   </si>
   <si>
@@ -712,18 +547,12 @@
     <t>Perez</t>
   </si>
   <si>
-    <t>NPerez@Coca-Cola.com</t>
-  </si>
-  <si>
     <t>Intern for Brand Marketing</t>
   </si>
   <si>
     <t>Thompson</t>
   </si>
   <si>
-    <t>Kelsey.Thompson@Nike.com</t>
-  </si>
-  <si>
     <t>International Marketing Executive | AI Evangelist | Top 50 Women Leaders in Georgia 2024 &amp; 2023</t>
   </si>
   <si>
@@ -731,15 +560,6 @@
   </si>
   <si>
     <t>Mumaw</t>
-  </si>
-  <si>
-    <t>KMumaw@Paypal.com</t>
-  </si>
-  <si>
-    <t>OLD EMAIL</t>
-  </si>
-  <si>
-    <t>MERGE STATUS</t>
   </si>
 </sst>
 </file>
@@ -815,135 +635,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9800"/>
-          <bgColor rgb="FFFF9800"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFA726"/>
-          <bgColor rgb="FFFFA726"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9800"/>
-          <bgColor rgb="FFFF9800"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFA726"/>
-          <bgColor rgb="FFFFA726"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6AA84F"/>
-          <bgColor rgb="FF6AA84F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1225,7 +917,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1243,12 +935,6 @@
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -1266,22 +952,18 @@
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -1289,482 +971,398 @@
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -1772,85 +1370,69 @@
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>121</v>
-      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>125</v>
-      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>128</v>
-      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>5</v>
@@ -1859,21 +1441,17 @@
         <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="2"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>131</v>
-      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
@@ -1882,395 +1460,327 @@
         <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="2"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>134</v>
-      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="2"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="2"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="2"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="2"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>149</v>
-      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="2"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>153</v>
-      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="2"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>156</v>
-      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="2"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>160</v>
-      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="2"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>164</v>
-      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="2"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>168</v>
-      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="2"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="2"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>175</v>
-      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="3"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="2"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>182</v>
+        <v>139</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>183</v>
-      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="2"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>188</v>
-      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="2"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="3"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>194</v>
+        <v>148</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>195</v>
+        <v>149</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="2"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>196</v>
-      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="3"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>198</v>
+        <v>151</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>7</v>
@@ -2278,200 +1788,164 @@
       <c r="E46" s="1"/>
       <c r="F46" s="2"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>199</v>
-      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="2"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>203</v>
-      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>205</v>
+        <v>156</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>206</v>
+        <v>157</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="2"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>207</v>
-      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="2"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>211</v>
-      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>213</v>
+        <v>162</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>214</v>
+        <v>163</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="2"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>215</v>
-      </c>
+      <c r="H50" s="1"/>
+      <c r="I50" s="3"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>218</v>
+        <v>166</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="2"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>219</v>
-      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>220</v>
+        <v>167</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="2"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>222</v>
-      </c>
+      <c r="H52" s="1"/>
+      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>224</v>
+        <v>170</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>225</v>
+        <v>171</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="2"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>226</v>
-      </c>
+      <c r="H53" s="1"/>
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>227</v>
+        <v>172</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="2"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>230</v>
-      </c>
+      <c r="H54" s="1"/>
+      <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>231</v>
+        <v>175</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
@@ -2480,40 +1954,32 @@
         <v>13</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>232</v>
+        <v>176</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="2"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>233</v>
-      </c>
+      <c r="H55" s="1"/>
+      <c r="I55" s="3"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="2"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>237</v>
-      </c>
+      <c r="H56" s="1"/>
+      <c r="I56" s="3"/>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
@@ -2680,9 +2146,6 @@
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{362A1A1E-926F-7044-8596-F29A08C1262E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>